<commit_message>
update some page of activity
</commit_message>
<xml_diff>
--- a/operate/src/main/resources/excel/activity_product_template.xlsx
+++ b/operate/src/main/resources/excel/activity_product_template.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guojiayu/code/uoms2/operate/src/main/resources/excel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="3435" windowWidth="28800" windowHeight="15675" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="活动商品列表" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">活动商品列表!$D$1:$D$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">活动商品列表!$D$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,94 +27,59 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>名称&lt;文本型&gt;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>非活动日常单价（元/件）&lt;数值型&gt;</t>
-    <rPh sb="0" eb="1">
-      <t>fei huo don</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>ri c</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>dan j</t>
-    </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>活动机制&lt;文本型&gt;</t>
-    <rPh sb="0" eb="1">
-      <t>huo don</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>ji zhi</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>wen ben xing</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>xing</t>
-    </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>活动通知体现最低单价（元/件）&lt;数值型&gt;</t>
-    <rPh sb="0" eb="1">
-      <t>huo don</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>tong zhi</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>ti</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>zui di</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>dan jia</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>yuan</t>
-    </rPh>
-    <rPh sb="13" eb="14">
-      <t>jian</t>
-    </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>活动期间体现最低单价（元/件）&lt;数值型&gt;</t>
-    <rPh sb="2" eb="3">
-      <t>qi j</t>
-    </rPh>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>商品ID&lt;文本型&gt;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>商品ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>商品名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日常商品单价
+（元/件）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>店铺活动机制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>满元减钱面额
+（元）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>立减金额
+（元）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>活动商品单价
+（元/件）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>满件打折
+（折）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>满元减钱门槛
+（元）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.00;[Red]0.00"/>
     <numFmt numFmtId="177" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="3">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="DengXian"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -124,6 +94,19 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -169,20 +152,20 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,56 +436,70 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="39.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.5" style="4" customWidth="1"/>
+    <col min="1" max="2" width="14" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" style="3" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9" s="7" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D1048576">
       <formula1>"活动价,满件打折,满元减钱,特价"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
+      <formula1>"满件打折,满元减钱,特价秒杀,预售付尾立减"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>